<commit_message>
Click en evento directo, empiezo ViewModel para ver Ingresos y Egresos en tabla
</commit_message>
<xml_diff>
--- a/AsistManager/wwwroot/Uploads/AsistManager.xlsx
+++ b/AsistManager/wwwroot/Uploads/AsistManager.xlsx
@@ -74,11 +74,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.6898876404"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7898876404"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.0898876404"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.8898876404"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.2898876404"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.0898876404"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.4898876404"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1898876404"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.9898876404"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.4898876404"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="4.1898876404"/>
   </cols>
@@ -128,30 +128,34 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Mercy</t>
+          <t>Reece</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Buchett</t>
+          <t>Shugg</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>33915209</v>
+        <v>12261987</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>45-00942068-77</t>
+          <t>06-25331652-11</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>828-928-1490</t>
-        </is>
-      </c>
-      <c r="F2" s="0"/>
+          <t>(142) 4993773</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Puku</t>
+        </is>
+      </c>
       <c r="G2" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="0" t="b">
         <v>0</v>
@@ -160,28 +164,32 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Kirbee</t>
+          <t>Selma</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Beaman</t>
+          <t>Gave</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>41206432</v>
+        <v>10149315</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>24-06194509-30</t>
+          <t>68-65597329-16</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>903-545-8993</t>
-        </is>
-      </c>
-      <c r="F3" s="0"/>
+          <t>(586) 8205499</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>Hartebeest, coke's</t>
+        </is>
+      </c>
       <c r="G3" s="0" t="b">
         <v>0</v>
       </c>
@@ -192,28 +200,32 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Charmain</t>
+          <t>Cobby</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Warret</t>
+          <t>Rogeon</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>12839337</v>
+        <v>8956649</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>31-34750684-78</t>
+          <t>17-13237035-61</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>828-810-0262</t>
-        </is>
-      </c>
-      <c r="F4" s="0"/>
+          <t>(382) 6611426</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Armadillo, common long-nosed</t>
+        </is>
+      </c>
       <c r="G4" s="0" t="b">
         <v>1</v>
       </c>
@@ -224,62 +236,70 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Val</t>
+          <t>Etti</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Buncher</t>
+          <t>Boulsher</t>
         </is>
       </c>
       <c r="C5" s="0" t="n">
-        <v>57899744</v>
+        <v>15572339</v>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>02-79318449-11</t>
+          <t>69-53131429-28</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>521-675-0851</t>
-        </is>
-      </c>
-      <c r="F5" s="0"/>
+          <t>(972) 6509150</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>Mongoose, banded</t>
+        </is>
+      </c>
       <c r="G5" s="0" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Sibella</t>
+          <t>Vinnie</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Healey</t>
+          <t>Pentony</t>
         </is>
       </c>
       <c r="C6" s="0" t="n">
-        <v>10354549</v>
+        <v>13354602</v>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>71-76585909-31</t>
+          <t>34-43197113-99</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>614-105-9543</t>
-        </is>
-      </c>
-      <c r="F6" s="0"/>
+          <t>(295) 8322970</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Ring-tailed coatimundi</t>
+        </is>
+      </c>
       <c r="G6" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="b">
         <v>1</v>
@@ -288,30 +308,34 @@
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>Cristionna</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Abramov</t>
+          <t>Billitteri</t>
         </is>
       </c>
       <c r="C7" s="0" t="n">
-        <v>48060066</v>
+        <v>81217729</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>79-03133813-69</t>
+          <t>26-80940595-96</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>414-406-4090</t>
-        </is>
-      </c>
-      <c r="F7" s="0"/>
+          <t>(775) 2516606</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>Eurasian beaver</t>
+        </is>
+      </c>
       <c r="G7" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="0" t="b">
         <v>0</v>
@@ -320,28 +344,32 @@
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Vernice</t>
+          <t>Ashlen</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Screach</t>
+          <t>de Tocqueville</t>
         </is>
       </c>
       <c r="C8" s="0" t="n">
-        <v>13978913</v>
+        <v>12436626</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>48-99394934-92</t>
+          <t>49-42574341-65</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>175-181-7272</t>
-        </is>
-      </c>
-      <c r="F8" s="0"/>
+          <t>(832) 8024500</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Greater blue-eared starling</t>
+        </is>
+      </c>
       <c r="G8" s="0" t="b">
         <v>0</v>
       </c>
@@ -352,92 +380,104 @@
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Harold</t>
+          <t>Alexis</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Shakelady</t>
+          <t>Damp</t>
         </is>
       </c>
       <c r="C9" s="0" t="n">
-        <v>65922087</v>
+        <v>91306638</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>99-15336833-53</t>
+          <t>67-34291374-92</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>463-641-9143</t>
-        </is>
-      </c>
-      <c r="F9" s="0"/>
+          <t>(883) 4920125</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>Mockingbird, galapagos</t>
+        </is>
+      </c>
       <c r="G9" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>Cirillo</t>
+          <t>Jeromy</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>McDonogh</t>
+          <t>Rielly</t>
         </is>
       </c>
       <c r="C10" s="0" t="n">
-        <v>42226601</v>
+        <v>29177523</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>80-60673786-52</t>
+          <t>20-93557794-67</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>307-992-4399</t>
-        </is>
-      </c>
-      <c r="F10" s="0"/>
+          <t>(792) 9271736</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Squirrel, indian giant</t>
+        </is>
+      </c>
       <c r="G10" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>Clarke</t>
+          <t>Garold</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Nelm</t>
+          <t>Reiner</t>
         </is>
       </c>
       <c r="C11" s="0" t="n">
-        <v>16559357</v>
+        <v>37647492</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>58-03066886-70</t>
+          <t>76-97691202-08</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>651-536-2457</t>
-        </is>
-      </c>
-      <c r="F11" s="0"/>
+          <t>(703) 5961604</t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>Goanna lizard</t>
+        </is>
+      </c>
       <c r="G11" s="0" t="b">
         <v>0</v>
       </c>
@@ -448,30 +488,34 @@
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>Donal</t>
+          <t>Stephen</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Fane</t>
+          <t>Danick</t>
         </is>
       </c>
       <c r="C12" s="0" t="n">
-        <v>87243355</v>
+        <v>78452955</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>19-76488265-20</t>
+          <t>63-57238603-93</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>155-256-7708</t>
-        </is>
-      </c>
-      <c r="F12" s="0"/>
+          <t>(329) 4881121</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Grey fox</t>
+        </is>
+      </c>
       <c r="G12" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="0" t="b">
         <v>1</v>
@@ -480,28 +524,32 @@
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>Lari</t>
+          <t>Hugibert</t>
         </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>de Chastelain</t>
+          <t>Bosomworth</t>
         </is>
       </c>
       <c r="C13" s="0" t="n">
-        <v>24973635</v>
+        <v>83756470</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>80-04057581-22</t>
+          <t>64-96350335-62</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>123-267-0293</t>
-        </is>
-      </c>
-      <c r="F13" s="0"/>
+          <t>(665) 3956554</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>African skink</t>
+        </is>
+      </c>
       <c r="G13" s="0" t="b">
         <v>1</v>
       </c>
@@ -512,28 +560,32 @@
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>Verina</t>
+          <t>Wanids</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>Presswell</t>
+          <t>Du Hamel</t>
         </is>
       </c>
       <c r="C14" s="0" t="n">
-        <v>80536505</v>
+        <v>93963919</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>24-29253307-08</t>
+          <t>50-91779460-40</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>755-568-5935</t>
-        </is>
-      </c>
-      <c r="F14" s="0"/>
+          <t>(407) 1366643</t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>Starfish, crown of thorns</t>
+        </is>
+      </c>
       <c r="G14" s="0" t="b">
         <v>1</v>
       </c>
@@ -544,28 +596,32 @@
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>Almeria</t>
+          <t>Demetria</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>Yedall</t>
+          <t>Wolledge</t>
         </is>
       </c>
       <c r="C15" s="0" t="n">
-        <v>70276787</v>
+        <v>82960998</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>51-03993333-58</t>
+          <t>59-13274709-91</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>811-565-4673</t>
-        </is>
-      </c>
-      <c r="F15" s="0"/>
+          <t>(883) 5654742</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>Square-lipped rhinoceros</t>
+        </is>
+      </c>
       <c r="G15" s="0" t="b">
         <v>1</v>
       </c>
@@ -576,92 +632,104 @@
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Delcine</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Rolstone</t>
+          <t>McMillan</t>
         </is>
       </c>
       <c r="C16" s="0" t="n">
-        <v>28860125</v>
+        <v>66144133</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>41-49826975-90</t>
+          <t>22-16911837-64</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>656-642-9067</t>
-        </is>
-      </c>
-      <c r="F16" s="0"/>
+          <t>(446) 2181833</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>Tyrant flycatcher</t>
+        </is>
+      </c>
       <c r="G16" s="0" t="b">
         <v>0</v>
       </c>
       <c r="H16" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>Britta</t>
+          <t>Shirline</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>Hattigan</t>
+          <t>Shelley</t>
         </is>
       </c>
       <c r="C17" s="0" t="n">
-        <v>5325809</v>
+        <v>41045523</v>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>69-08377604-57</t>
+          <t>55-11757474-60</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>874-525-2813</t>
-        </is>
-      </c>
-      <c r="F17" s="0"/>
+          <t>(378) 8226608</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>Puffin, horned</t>
+        </is>
+      </c>
       <c r="G17" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>Devondra</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>Aubin</t>
+          <t>Grieger</t>
         </is>
       </c>
       <c r="C18" s="0" t="n">
-        <v>89189768</v>
+        <v>56792120</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>03-23917447-08</t>
+          <t>34-62192081-13</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>133-881-4163</t>
-        </is>
-      </c>
-      <c r="F18" s="0"/>
+          <t>(533) 5560622</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>Drongo, fork-tailed</t>
+        </is>
+      </c>
       <c r="G18" s="0" t="b">
         <v>0</v>
       </c>
@@ -672,30 +740,34 @@
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>Morris</t>
+          <t>Calv</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>Tipperton</t>
+          <t>Gobourn</t>
         </is>
       </c>
       <c r="C19" s="0" t="n">
-        <v>86538156</v>
+        <v>32833883</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>25-88373280-89</t>
+          <t>90-22862581-96</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>768-772-7447</t>
-        </is>
-      </c>
-      <c r="F19" s="0"/>
+          <t>(568) 4775056</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>Cat, african wild</t>
+        </is>
+      </c>
       <c r="G19" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="0" t="b">
         <v>0</v>
@@ -704,30 +776,34 @@
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>Larry</t>
+          <t>Haleigh</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Banger</t>
+          <t>Godlee</t>
         </is>
       </c>
       <c r="C20" s="0" t="n">
-        <v>57723001</v>
+        <v>8893982</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>14-55450166-68</t>
+          <t>42-77773577-94</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>867-265-6252</t>
-        </is>
-      </c>
-      <c r="F20" s="0"/>
+          <t>(626) 8553839</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>Oriental short-clawed otter</t>
+        </is>
+      </c>
       <c r="G20" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="0" t="b">
         <v>1</v>
@@ -736,60 +812,68 @@
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>Dulsea</t>
+          <t>Todd</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>Tolson</t>
+          <t>Chree</t>
         </is>
       </c>
       <c r="C21" s="0" t="n">
-        <v>34638291</v>
+        <v>71262655</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>64-89872039-70</t>
+          <t>95-14518863-58</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>880-146-6793</t>
-        </is>
-      </c>
-      <c r="F21" s="0"/>
+          <t>(772) 2582295</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>Starling, superb</t>
+        </is>
+      </c>
       <c r="G21" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H21" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>Amata</t>
+          <t>Kane</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>Fielders</t>
+          <t>Dole</t>
         </is>
       </c>
       <c r="C22" s="0" t="n">
-        <v>37911713</v>
+        <v>2801641</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>06-45170396-95</t>
+          <t>32-56096304-96</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>385-194-9033</t>
-        </is>
-      </c>
-      <c r="F22" s="0"/>
+          <t>(464) 2533904</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>Caiman, spectacled</t>
+        </is>
+      </c>
       <c r="G22" s="0" t="b">
         <v>1</v>
       </c>
@@ -800,30 +884,34 @@
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>Annmaria</t>
+          <t>Alvan</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Arnot</t>
+          <t>Mingaud</t>
         </is>
       </c>
       <c r="C23" s="0" t="n">
-        <v>64678066</v>
+        <v>89691387</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>30-88444511-47</t>
+          <t>00-09784203-93</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>637-224-3095</t>
-        </is>
-      </c>
-      <c r="F23" s="0"/>
+          <t>(239) 6220253</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>Monster, gila</t>
+        </is>
+      </c>
       <c r="G23" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="0" t="b">
         <v>0</v>
@@ -832,30 +920,34 @@
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>Jillie</t>
+          <t>Liam</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Bamber</t>
+          <t>Wakeham</t>
         </is>
       </c>
       <c r="C24" s="0" t="n">
-        <v>43458611</v>
+        <v>33673900</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>00-48408675-02</t>
+          <t>93-58645938-93</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>511-271-1578</t>
-        </is>
-      </c>
-      <c r="F24" s="0"/>
+          <t>(297) 5042126</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>Numbat</t>
+        </is>
+      </c>
       <c r="G24" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="0" t="b">
         <v>0</v>
@@ -864,65 +956,73 @@
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>Grazia</t>
+          <t>Tasia</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Phillott</t>
+          <t>Gaven</t>
         </is>
       </c>
       <c r="C25" s="0" t="n">
-        <v>85309759</v>
+        <v>91546708</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>60-41885078-50</t>
+          <t>72-78884924-07</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>366-321-0461</t>
-        </is>
-      </c>
-      <c r="F25" s="0"/>
+          <t>(645) 1485584</t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>Tortoise, indian star</t>
+        </is>
+      </c>
       <c r="G25" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>Gerrie</t>
+          <t>Silvan</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Stanlack</t>
+          <t>Nealand</t>
         </is>
       </c>
       <c r="C26" s="0" t="n">
-        <v>74690157</v>
+        <v>51815122</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>80-61942212-30</t>
+          <t>61-93615499-36</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>451-996-0602</t>
-        </is>
-      </c>
-      <c r="F26" s="0"/>
+          <t>(876) 6153539</t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>Ibis, puna</t>
+        </is>
+      </c>
       <c r="G26" s="0" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>